<commit_message>
[stage 4] bot deploy
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Номер заказа</t>
   </si>
@@ -62,9 +62,6 @@
   </si>
   <si>
     <t>Не закрыт</t>
-  </si>
-  <si>
-    <t>123 сбер</t>
   </si>
 </sst>
 </file>
@@ -436,34 +433,34 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="B2">
-        <v>732832293</v>
+        <v>185404885</v>
       </c>
       <c r="C2">
-        <v>21315345</v>
+        <v>236322856</v>
       </c>
       <c r="D2" s="2">
-        <v>44807.443978703704</v>
+        <v>45041.86893779451</v>
       </c>
       <c r="E2">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="F2" s="2">
-        <v>44818.77747765046</v>
+        <v>45041.50833333333</v>
       </c>
       <c r="G2">
-        <v>500</v>
+        <v>1212</v>
       </c>
       <c r="H2">
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="I2">
-        <v>450</v>
+        <v>121</v>
       </c>
       <c r="J2">
-        <v>50</v>
+        <v>1090</v>
       </c>
       <c r="K2" t="s">
         <v>13</v>
@@ -474,154 +471,230 @@
     </row>
     <row r="3">
       <c r="A3">
+        <v>24</v>
+      </c>
+      <c r="B3">
+        <v>185404885</v>
+      </c>
+      <c r="C3">
+        <v>236322856</v>
+      </c>
+      <c r="D3" s="2">
+        <v>45041.883623359245</v>
+      </c>
+      <c r="E3">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>456456</v>
-      </c>
-      <c r="C3">
-        <v>9680670</v>
-      </c>
-      <c r="D3" s="2">
-        <v>44835.611745462964</v>
-      </c>
-      <c r="E3">
-        <v>11</v>
-      </c>
       <c r="F3" s="2">
-        <v>44836.6118491088</v>
+        <v>45041.50833333333</v>
       </c>
       <c r="G3">
-        <v>1000</v>
+        <v>1200</v>
       </c>
       <c r="H3">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="I3">
-        <v>800</v>
+        <v>120</v>
       </c>
       <c r="J3">
-        <v>200</v>
+        <v>1080</v>
       </c>
       <c r="K3" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="3" t="s">
-        <v>15</v>
+      <c r="L3" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="B4">
-        <v>5645647</v>
+        <v>185404885</v>
       </c>
       <c r="C4">
-        <v>11123233</v>
+        <v>0</v>
       </c>
       <c r="D4" s="2">
-        <v>44696.613132673614</v>
+        <v>45041.886526336224</v>
       </c>
       <c r="E4">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="F4" s="2">
-        <v>44744.61322702546</v>
+        <v>45041.50833333333</v>
       </c>
       <c r="G4">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>92</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>4600</v>
+        <v>0</v>
       </c>
       <c r="J4">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="K4" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>14</v>
+      <c r="L4" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="B5">
-        <v>123123</v>
+        <v>185404885</v>
       </c>
       <c r="C5">
-        <v>5768655</v>
+        <v>0</v>
       </c>
       <c r="D5" s="2">
-        <v>44868.61496076389</v>
+        <v>45042.84731792426</v>
       </c>
       <c r="E5">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="F5" s="2">
-        <v>44884.615064652775</v>
+        <v>45049.50833333333</v>
       </c>
       <c r="G5">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>98</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>196</v>
+        <v>0</v>
       </c>
       <c r="J5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K5" t="s">
         <v>13</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>14</v>
+      <c r="L5" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="B6">
-        <v>236322856</v>
+        <v>185404885</v>
       </c>
       <c r="C6">
-        <v>236322856</v>
+        <v>0</v>
       </c>
       <c r="D6" s="2">
-        <v>44746.61244488426</v>
+        <v>45042.86098662064</v>
       </c>
       <c r="E6">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F6" s="2">
-        <v>44749.61254543981</v>
+        <v>45043.50833333333</v>
       </c>
       <c r="G6">
-        <v>350</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>95</v>
+        <v>0</v>
       </c>
       <c r="I6">
-        <v>332</v>
+        <v>0</v>
       </c>
       <c r="J6">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L6" s="3" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>28</v>
+      </c>
+      <c r="B7">
+        <v>185404885</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>45042.86229964735</v>
+      </c>
+      <c r="E7">
+        <v>12</v>
+      </c>
+      <c r="F7" s="2">
+        <v>45056.50833333333</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>22</v>
+      </c>
+      <c r="B8">
+        <v>185404885</v>
+      </c>
+      <c r="C8">
+        <v>236322856</v>
+      </c>
+      <c r="D8" s="2">
+        <v>45041.86554414516</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8" s="2">
+        <v>45041.50833333333</v>
+      </c>
+      <c r="G8">
+        <v>234</v>
+      </c>
+      <c r="H8">
+        <v>10</v>
+      </c>
+      <c r="I8">
+        <v>23</v>
+      </c>
+      <c r="J8">
+        <v>210</v>
+      </c>
+      <c r="K8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>